<commit_message>
102824 1114PM from PC
</commit_message>
<xml_diff>
--- a/2024/Fall 2024/TFES Lab/Airfoil/Airfoil_DataSheet.xlsx
+++ b/2024/Fall 2024/TFES Lab/Airfoil/Airfoil_DataSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyl\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brand\Documents\SchoolFiles\2024\Fall 2024\TFES Lab\Airfoil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BA0ED2-3E47-4F41-81D4-FA51B6316AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B940064-F27A-47CA-B51C-62855D16AEED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020" sheetId="4" r:id="rId1"/>
@@ -1095,12 +1095,164 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1116,24 +1268,12 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1154,146 +1294,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4107,13 +4107,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>55379</xdr:colOff>
+      <xdr:colOff>45854</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>30939</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1154225</xdr:colOff>
+      <xdr:colOff>1039925</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>321341</xdr:rowOff>
     </xdr:to>
@@ -4130,8 +4130,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7935286" y="7881311"/>
-          <a:ext cx="1098846" cy="290402"/>
+          <a:off x="6875279" y="7860489"/>
+          <a:ext cx="994071" cy="290402"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6441,67 +6441,66 @@
   </sheetPr>
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16:J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="2.77734375" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
-    <col min="7" max="8" width="14.77734375" customWidth="1"/>
-    <col min="9" max="9" width="2.77734375" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" customWidth="1"/>
-    <col min="11" max="11" width="9.77734375" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" customWidth="1"/>
-    <col min="13" max="13" width="15.77734375" customWidth="1"/>
-    <col min="14" max="14" width="3.33203125" style="9" customWidth="1"/>
-    <col min="15" max="16" width="10.6640625" customWidth="1"/>
-    <col min="17" max="17" width="7.33203125" customWidth="1"/>
-    <col min="18" max="20" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="2.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="12" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="3.28515625" style="9" customWidth="1"/>
+    <col min="15" max="16" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="7.28515625" customWidth="1"/>
+    <col min="18" max="20" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28.2">
-      <c r="A1" s="78" t="s">
+    <row r="1" spans="1:14" ht="27.75">
+      <c r="A1" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
       <c r="J1" s="12"/>
       <c r="K1" s="24"/>
       <c r="L1" s="24"/>
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
     </row>
-    <row r="2" spans="1:14" ht="22.8">
-      <c r="A2" s="79" t="s">
+    <row r="2" spans="1:14" ht="23.25">
+      <c r="A2" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
       <c r="J2" s="13"/>
       <c r="K2" s="25"/>
       <c r="L2" s="25"/>
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
     </row>
-    <row r="3" spans="1:14" ht="21">
+    <row r="3" spans="1:14" ht="20.25">
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="J3" s="9"/>
@@ -6569,162 +6568,162 @@
       <c r="K7" s="9"/>
       <c r="N7"/>
     </row>
-    <row r="8" spans="1:14" ht="28.05" customHeight="1" thickTop="1">
-      <c r="A8" s="81" t="s">
+    <row r="8" spans="1:14" ht="28.15" customHeight="1" thickTop="1">
+      <c r="A8" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="96"/>
-      <c r="F8" s="81" t="s">
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="64"/>
+      <c r="F8" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="82"/>
-      <c r="H8" s="83"/>
-      <c r="J8" s="81" t="s">
+      <c r="G8" s="95"/>
+      <c r="H8" s="96"/>
+      <c r="J8" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="84"/>
-      <c r="L8" s="82"/>
-      <c r="M8" s="83"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="95"/>
+      <c r="M8" s="96"/>
       <c r="N8"/>
     </row>
     <row r="9" spans="1:14" ht="30" customHeight="1" thickBot="1">
-      <c r="A9" s="97" t="s">
+      <c r="A9" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="98"/>
-      <c r="C9" s="98"/>
-      <c r="D9" s="99"/>
-      <c r="F9" s="93" t="s">
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="67"/>
+      <c r="F9" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="121"/>
-      <c r="H9" s="122"/>
-      <c r="J9" s="93" t="s">
+      <c r="G9" s="89"/>
+      <c r="H9" s="90"/>
+      <c r="J9" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
-      <c r="M9" s="95"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="57"/>
       <c r="N9"/>
     </row>
-    <row r="10" spans="1:14" ht="28.05" customHeight="1" thickTop="1">
-      <c r="A10" s="100" t="s">
+    <row r="10" spans="1:14" ht="28.15" customHeight="1" thickTop="1">
+      <c r="A10" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="102"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="70"/>
       <c r="F10" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="89" t="s">
+      <c r="G10" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="90"/>
-      <c r="J10" s="117"/>
-      <c r="K10" s="118"/>
-      <c r="L10" s="110" t="s">
+      <c r="H10" s="98"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="86"/>
+      <c r="L10" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="111"/>
+      <c r="M10" s="79"/>
       <c r="N10"/>
     </row>
-    <row r="11" spans="1:14" ht="28.05" customHeight="1">
+    <row r="11" spans="1:14" ht="28.15" customHeight="1">
       <c r="A11" s="36"/>
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="103"/>
-      <c r="D11" s="104"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="72"/>
       <c r="F11" s="18">
         <v>0</v>
       </c>
-      <c r="G11" s="91"/>
-      <c r="H11" s="92"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="120"/>
-      <c r="L11" s="112" t="s">
+      <c r="G11" s="99"/>
+      <c r="H11" s="100"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="88"/>
+      <c r="L11" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="M11" s="113"/>
+      <c r="M11" s="81"/>
       <c r="N11"/>
     </row>
-    <row r="12" spans="1:14" ht="28.05" customHeight="1" thickBot="1">
+    <row r="12" spans="1:14" ht="28.15" customHeight="1" thickBot="1">
       <c r="A12" s="37"/>
-      <c r="B12" s="105" t="s">
+      <c r="B12" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="105"/>
-      <c r="D12" s="106"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="74"/>
       <c r="F12" s="18">
         <v>1</v>
       </c>
-      <c r="G12" s="55"/>
-      <c r="H12" s="56"/>
-      <c r="J12" s="114"/>
-      <c r="K12" s="115"/>
-      <c r="L12" s="115"/>
-      <c r="M12" s="116"/>
+      <c r="G12" s="101"/>
+      <c r="H12" s="102"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="84"/>
       <c r="N12"/>
     </row>
-    <row r="13" spans="1:14" ht="28.05" customHeight="1" thickTop="1">
-      <c r="A13" s="107"/>
-      <c r="B13" s="108"/>
-      <c r="C13" s="108"/>
-      <c r="D13" s="109"/>
+    <row r="13" spans="1:14" ht="28.15" customHeight="1" thickTop="1">
+      <c r="A13" s="75"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="77"/>
       <c r="F13" s="18">
         <v>2</v>
       </c>
-      <c r="G13" s="55"/>
-      <c r="H13" s="56"/>
-      <c r="J13" s="85" t="s">
+      <c r="G13" s="101"/>
+      <c r="H13" s="102"/>
+      <c r="J13" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="K13" s="86"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="88"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="61"/>
       <c r="N13"/>
     </row>
-    <row r="14" spans="1:14" ht="28.05" customHeight="1">
-      <c r="A14" s="68" t="s">
+    <row r="14" spans="1:14" ht="28.15" customHeight="1">
+      <c r="A14" s="116" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="69"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="73" t="s">
+      <c r="B14" s="117"/>
+      <c r="C14" s="109"/>
+      <c r="D14" s="121" t="s">
         <v>21</v>
       </c>
       <c r="F14" s="18">
         <v>3</v>
       </c>
-      <c r="G14" s="55"/>
-      <c r="H14" s="56"/>
-      <c r="J14" s="65" t="s">
+      <c r="G14" s="101"/>
+      <c r="H14" s="102"/>
+      <c r="J14" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="59" t="s">
+      <c r="K14" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="L14" s="57" t="s">
+      <c r="L14" s="109" t="s">
         <v>30</v>
       </c>
-      <c r="M14" s="58"/>
+      <c r="M14" s="110"/>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:14" ht="28.05" customHeight="1" thickBot="1">
-      <c r="A15" s="70"/>
-      <c r="B15" s="71"/>
-      <c r="C15" s="72"/>
-      <c r="D15" s="74"/>
+    <row r="15" spans="1:14" ht="28.15" customHeight="1" thickBot="1">
+      <c r="A15" s="118"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="120"/>
+      <c r="D15" s="122"/>
       <c r="F15" s="18">
         <v>4</v>
       </c>
-      <c r="G15" s="55"/>
-      <c r="H15" s="56"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="60"/>
+      <c r="G15" s="101"/>
+      <c r="H15" s="102"/>
+      <c r="J15" s="115"/>
+      <c r="K15" s="112"/>
       <c r="L15" s="49" t="s">
         <v>25</v>
       </c>
@@ -6733,18 +6732,18 @@
       </c>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" ht="28.05" customHeight="1" thickTop="1">
-      <c r="A16" s="75" t="s">
+    <row r="16" spans="1:14" ht="28.15" customHeight="1" thickTop="1">
+      <c r="A16" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="75"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="103"/>
+      <c r="D16" s="103"/>
       <c r="F16" s="18">
         <v>5</v>
       </c>
-      <c r="G16" s="55"/>
-      <c r="H16" s="56"/>
+      <c r="G16" s="101"/>
+      <c r="H16" s="102"/>
       <c r="I16" s="14"/>
       <c r="J16" s="29">
         <v>0.05</v>
@@ -6756,18 +6755,18 @@
       <c r="M16" s="48"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="1:15" ht="28.05" customHeight="1">
-      <c r="A17" s="67" t="s">
+    <row r="17" spans="1:15" ht="28.15" customHeight="1">
+      <c r="A17" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="67"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
+      <c r="B17" s="104"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="104"/>
       <c r="F17" s="18">
         <v>6</v>
       </c>
-      <c r="G17" s="55"/>
-      <c r="H17" s="56"/>
+      <c r="G17" s="101"/>
+      <c r="H17" s="102"/>
       <c r="I17" s="14"/>
       <c r="J17" s="18">
         <v>0.1</v>
@@ -6779,18 +6778,18 @@
       <c r="M17" s="41"/>
       <c r="N17"/>
     </row>
-    <row r="18" spans="1:15" ht="28.05" customHeight="1">
-      <c r="A18" s="61" t="s">
+    <row r="18" spans="1:15" ht="28.15" customHeight="1">
+      <c r="A18" s="113" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="62"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
+      <c r="B18" s="92"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
       <c r="F18" s="18">
         <v>7</v>
       </c>
-      <c r="G18" s="55"/>
-      <c r="H18" s="56"/>
+      <c r="G18" s="101"/>
+      <c r="H18" s="102"/>
       <c r="I18" s="14"/>
       <c r="J18" s="18">
         <v>0.2</v>
@@ -6802,12 +6801,12 @@
       <c r="M18" s="41"/>
       <c r="N18"/>
     </row>
-    <row r="19" spans="1:15" ht="28.05" customHeight="1">
+    <row r="19" spans="1:15" ht="28.15" customHeight="1">
       <c r="F19" s="18">
         <v>8</v>
       </c>
-      <c r="G19" s="55"/>
-      <c r="H19" s="56"/>
+      <c r="G19" s="101"/>
+      <c r="H19" s="102"/>
       <c r="I19" s="7"/>
       <c r="J19" s="18">
         <v>0.3</v>
@@ -6819,12 +6818,12 @@
       <c r="M19" s="41"/>
       <c r="N19" s="1"/>
     </row>
-    <row r="20" spans="1:15" ht="28.05" customHeight="1">
+    <row r="20" spans="1:15" ht="28.15" customHeight="1">
       <c r="F20" s="18">
         <v>9</v>
       </c>
-      <c r="G20" s="55"/>
-      <c r="H20" s="56"/>
+      <c r="G20" s="101"/>
+      <c r="H20" s="102"/>
       <c r="I20" s="2"/>
       <c r="J20" s="18">
         <v>0.4</v>
@@ -6836,12 +6835,12 @@
       <c r="M20" s="41"/>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:15" ht="28.05" customHeight="1">
+    <row r="21" spans="1:15" ht="28.15" customHeight="1">
       <c r="F21" s="18">
         <v>10</v>
       </c>
-      <c r="G21" s="55"/>
-      <c r="H21" s="56"/>
+      <c r="G21" s="101"/>
+      <c r="H21" s="102"/>
       <c r="I21" s="2"/>
       <c r="J21" s="18">
         <v>0.5</v>
@@ -6853,12 +6852,12 @@
       <c r="M21" s="41"/>
       <c r="N21" s="1"/>
     </row>
-    <row r="22" spans="1:15" ht="28.05" customHeight="1">
+    <row r="22" spans="1:15" ht="28.15" customHeight="1">
       <c r="F22" s="18">
         <v>11</v>
       </c>
-      <c r="G22" s="55"/>
-      <c r="H22" s="56"/>
+      <c r="G22" s="101"/>
+      <c r="H22" s="102"/>
       <c r="I22" s="2"/>
       <c r="J22" s="18">
         <v>0.6</v>
@@ -6871,12 +6870,12 @@
       <c r="N22" s="1"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" ht="28.05" customHeight="1">
+    <row r="23" spans="1:15" ht="28.15" customHeight="1">
       <c r="F23" s="18">
         <v>12</v>
       </c>
-      <c r="G23" s="63"/>
-      <c r="H23" s="64"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="106"/>
       <c r="I23" s="2"/>
       <c r="J23" s="18">
         <v>0.7</v>
@@ -6889,12 +6888,12 @@
       <c r="N23" s="2"/>
       <c r="O23" s="3"/>
     </row>
-    <row r="24" spans="1:15" ht="28.05" customHeight="1" thickBot="1">
+    <row r="24" spans="1:15" ht="28.15" customHeight="1" thickBot="1">
       <c r="F24" s="19">
         <v>13</v>
       </c>
-      <c r="G24" s="63"/>
-      <c r="H24" s="64"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="106"/>
       <c r="I24" s="2"/>
       <c r="J24" s="19">
         <v>0.8</v>
@@ -6907,57 +6906,57 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:15" ht="28.05" customHeight="1" thickTop="1">
+    <row r="25" spans="1:15" ht="28.15" customHeight="1" thickTop="1">
       <c r="F25" s="18">
         <v>14</v>
       </c>
-      <c r="G25" s="63"/>
-      <c r="H25" s="64"/>
+      <c r="G25" s="105"/>
+      <c r="H25" s="106"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="85" t="s">
+      <c r="J25" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="K25" s="86"/>
-      <c r="L25" s="87"/>
-      <c r="M25" s="88"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="61"/>
       <c r="N25" s="5"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" spans="1:15" ht="28.05" customHeight="1">
+    <row r="26" spans="1:15" ht="28.15" customHeight="1">
       <c r="B26" s="31"/>
       <c r="C26" s="31"/>
       <c r="D26" s="31"/>
       <c r="F26" s="18">
         <v>15</v>
       </c>
-      <c r="G26" s="63"/>
-      <c r="H26" s="64"/>
+      <c r="G26" s="105"/>
+      <c r="H26" s="106"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="65" t="s">
+      <c r="J26" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="K26" s="59" t="s">
+      <c r="K26" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="L26" s="57" t="s">
+      <c r="L26" s="109" t="s">
         <v>30</v>
       </c>
-      <c r="M26" s="58"/>
+      <c r="M26" s="110"/>
       <c r="N26" s="4"/>
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="1:15" ht="28.05" customHeight="1" thickBot="1">
+    <row r="27" spans="1:15" ht="28.15" customHeight="1" thickBot="1">
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
       <c r="D27" s="32"/>
       <c r="F27" s="20">
         <v>16</v>
       </c>
-      <c r="G27" s="76"/>
-      <c r="H27" s="77"/>
+      <c r="G27" s="107"/>
+      <c r="H27" s="108"/>
       <c r="I27" s="2"/>
-      <c r="J27" s="66"/>
-      <c r="K27" s="60"/>
+      <c r="J27" s="115"/>
+      <c r="K27" s="112"/>
       <c r="L27" s="49" t="s">
         <v>25</v>
       </c>
@@ -6967,15 +6966,15 @@
       <c r="N27" s="3"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="1:15" ht="28.05" customHeight="1" thickTop="1">
+    <row r="28" spans="1:15" ht="28.15" customHeight="1" thickTop="1">
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
       <c r="D28" s="32"/>
-      <c r="F28" s="75" t="s">
+      <c r="F28" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="75"/>
-      <c r="H28" s="75"/>
+      <c r="G28" s="103"/>
+      <c r="H28" s="103"/>
       <c r="I28" s="2"/>
       <c r="J28" s="29">
         <v>0.05</v>
@@ -6988,15 +6987,15 @@
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="1:15" ht="28.05" customHeight="1">
+    <row r="29" spans="1:15" ht="28.15" customHeight="1">
       <c r="B29" s="31"/>
       <c r="C29" s="31"/>
       <c r="D29" s="31"/>
-      <c r="F29" s="67" t="s">
+      <c r="F29" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="G29" s="67"/>
-      <c r="H29" s="67"/>
+      <c r="G29" s="104"/>
+      <c r="H29" s="104"/>
       <c r="I29" s="2"/>
       <c r="J29" s="18">
         <v>0.1</v>
@@ -7009,7 +7008,7 @@
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="1:15" ht="28.05" customHeight="1">
+    <row r="30" spans="1:15" ht="28.15" customHeight="1">
       <c r="F30" s="32"/>
       <c r="G30" s="32"/>
       <c r="H30" s="32"/>
@@ -7025,7 +7024,7 @@
       <c r="N30" s="6"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="1:15" ht="28.05" customHeight="1">
+    <row r="31" spans="1:15" ht="28.15" customHeight="1">
       <c r="E31" s="2"/>
       <c r="F31" s="32"/>
       <c r="G31" s="32"/>
@@ -7041,7 +7040,7 @@
       <c r="M31" s="41"/>
       <c r="N31"/>
     </row>
-    <row r="32" spans="1:15" ht="28.05" customHeight="1">
+    <row r="32" spans="1:15" ht="28.15" customHeight="1">
       <c r="E32" s="2"/>
       <c r="F32" s="31"/>
       <c r="G32" s="31"/>
@@ -7057,7 +7056,7 @@
       <c r="M32" s="41"/>
       <c r="N32"/>
     </row>
-    <row r="33" spans="6:14" ht="28.05" customHeight="1">
+    <row r="33" spans="6:14" ht="28.15" customHeight="1">
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
       <c r="H33" s="30"/>
@@ -7072,7 +7071,7 @@
       <c r="M33" s="41"/>
       <c r="N33"/>
     </row>
-    <row r="34" spans="6:14" ht="28.05" customHeight="1">
+    <row r="34" spans="6:14" ht="28.15" customHeight="1">
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
       <c r="H34" s="30"/>
@@ -7087,7 +7086,7 @@
       <c r="M34" s="41"/>
       <c r="N34"/>
     </row>
-    <row r="35" spans="6:14" ht="28.05" customHeight="1">
+    <row r="35" spans="6:14" ht="28.15" customHeight="1">
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
       <c r="H35" s="30"/>
@@ -7102,7 +7101,7 @@
       <c r="M35" s="41"/>
       <c r="N35"/>
     </row>
-    <row r="36" spans="6:14" ht="28.05" customHeight="1" thickBot="1">
+    <row r="36" spans="6:14" ht="28.15" customHeight="1" thickBot="1">
       <c r="I36" s="32"/>
       <c r="J36" s="20">
         <v>0.8</v>
@@ -7114,7 +7113,7 @@
       <c r="M36" s="47"/>
       <c r="N36"/>
     </row>
-    <row r="37" spans="6:14" ht="46.05" customHeight="1" thickTop="1">
+    <row r="37" spans="6:14" ht="46.15" customHeight="1" thickTop="1">
       <c r="I37" s="32"/>
       <c r="J37" s="27"/>
       <c r="K37" s="27"/>
@@ -7122,42 +7121,49 @@
       <c r="M37" s="28"/>
       <c r="N37"/>
     </row>
-    <row r="38" spans="6:14" ht="31.95" customHeight="1">
+    <row r="38" spans="6:14" ht="31.9" customHeight="1">
       <c r="I38" s="31"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="N38"/>
     </row>
-    <row r="39" spans="6:14" ht="16.95" customHeight="1">
+    <row r="39" spans="6:14" ht="16.899999999999999" customHeight="1">
       <c r="I39" s="21"/>
       <c r="N39"/>
     </row>
-    <row r="40" spans="6:14" ht="16.95" customHeight="1">
+    <row r="40" spans="6:14" ht="16.899999999999999" customHeight="1">
       <c r="N40"/>
     </row>
-    <row r="41" spans="6:14" ht="22.05" customHeight="1">
+    <row r="41" spans="6:14" ht="22.15" customHeight="1">
       <c r="N41" s="28"/>
     </row>
-    <row r="42" spans="6:14" ht="22.05" customHeight="1"/>
+    <row r="42" spans="6:14" ht="22.15" customHeight="1"/>
     <row r="43" spans="6:14" ht="27" customHeight="1"/>
     <row r="44" spans="6:14" ht="27" customHeight="1"/>
     <row r="45" spans="6:14" ht="27" customHeight="1"/>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G27:H27"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="F8:H8"/>
@@ -7174,34 +7180,27 @@
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.49" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
-  <pageSetup scale="62" orientation="portrait"/>
+  <pageSetup scale="62" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="14" max="31" man="1"/>
   </colBreaks>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>